<commit_message>
Updated BGR_grids model - 2025-08-14 00:57
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR_grids/SubRES_Tmpl/SubRES_REZoning_Sol_Win_and_Hydro.xlsx
+++ b/VerveStacks_BGR_grids/SubRES_Tmpl/SubRES_REZoning_Sol_Win_and_Hydro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8083A31-CAF9-4F70-9406-DC495737C725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B530433-74CB-4ECB-8F3A-BD080C0B6338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4199,7 +4199,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E6E70CF-C739-2D7C-9DCF-0576C26A80BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B8B57FB-936E-55A3-084C-95CFF31B53FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4254,7 +4254,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85435EC3-9BA9-20DE-78F6-3375554AE443}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{307C2F10-EE7B-41E7-13E1-A4C88775ABA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4309,7 +4309,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5DC6C48-43F7-FCDA-9849-9D47BDFD4BD7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2887230-29ED-44C8-BF5B-15BD1DA96A12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6812,7 +6812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCD97C0-8B94-4F9B-85BE-A5C6716B9E81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AE177F-9AC6-4B79-A681-BE1751CF06EF}">
   <dimension ref="A1:AG161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12958,7 +12958,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E610079F-D4DD-4112-BBD5-DFE1AAC6EEF0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1CD47C-D7FD-4B38-914A-4EDD8C05532A}">
   <dimension ref="A1:O159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>